<commit_message>
Upgrade with new parameter
Upgrade with new parameter
</commit_message>
<xml_diff>
--- a/LSTM/600233.xlsx
+++ b/LSTM/600233.xlsx
@@ -398,7 +398,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G287"/>
+  <dimension ref="A1:G288"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -6990,19 +6990,42 @@
         <v>12.60999965667725</v>
       </c>
       <c r="C287">
-        <v>13.19999980926514</v>
+        <v>13.32999992370605</v>
       </c>
       <c r="D287">
         <v>12.5600004196167</v>
       </c>
       <c r="E287">
+        <v>13.30000019073486</v>
+      </c>
+      <c r="F287">
+        <v>13.30000019073486</v>
+      </c>
+      <c r="G287">
+        <v>22529806</v>
+      </c>
+    </row>
+    <row r="288" spans="1:7">
+      <c r="A288" s="2">
+        <v>45363</v>
+      </c>
+      <c r="B288">
         <v>13.14999961853027</v>
       </c>
-      <c r="F287">
-        <v>13.14999961853027</v>
-      </c>
-      <c r="G287">
-        <v>14133384</v>
+      <c r="C288">
+        <v>14.05000019073486</v>
+      </c>
+      <c r="D288">
+        <v>13</v>
+      </c>
+      <c r="E288">
+        <v>13.94999980926514</v>
+      </c>
+      <c r="F288">
+        <v>13.94999980926514</v>
+      </c>
+      <c r="G288">
+        <v>25657155</v>
       </c>
     </row>
   </sheetData>

</xml_diff>